<commit_message>
Update snowballing with authors' answers
</commit_message>
<xml_diff>
--- a/notebooks/output/gathering.xlsx
+++ b/notebooks/output/gathering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="123">
   <si>
     <t>Annotations</t>
   </si>
@@ -152,18 +152,30 @@
     <t>Excl</t>
   </si>
   <si>
-    <t>For Provenance</t>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Prov</t>
+  </si>
+  <si>
+    <t>Defi</t>
+  </si>
+  <si>
+    <t>Necessity</t>
+  </si>
+  <si>
+    <t>Opt</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>Passive Monitoring</t>
   </si>
   <si>
     <t>✓</t>
   </si>
   <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>Passive Monitoring</t>
-  </si>
-  <si>
     <t>Overriding</t>
   </si>
   <si>
@@ -242,15 +254,15 @@
     <t>SisGExp</t>
   </si>
   <si>
+    <t>SPADE</t>
+  </si>
+  <si>
     <t>StarFlow</t>
   </si>
   <si>
     <t>Sumatra</t>
   </si>
   <si>
-    <t>Tariq, Ali, and Gehani</t>
-  </si>
-  <si>
     <t>Variolite</t>
   </si>
   <si>
@@ -278,88 +290,97 @@
     <t xml:space="preserve"> \citet{michaelides2016a}</t>
   </si>
   <si>
-    <t xml:space="preserve"> \citet{tariq2012a}</t>
-  </si>
-  <si>
     <t>User defined, Attributes, Files (I/O), Parameters, Source</t>
   </si>
   <si>
     <t>Commands, Variables, Random Seed</t>
   </si>
   <si>
+    <t>User defined, Files, Platform</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Commands, Variables, Random Seed, Files (I)</t>
+  </si>
+  <si>
+    <t>User defined, Parameters, Platform, Modules</t>
+  </si>
+  <si>
+    <t>Files (I/O - metadata)</t>
+  </si>
+  <si>
+    <t>User defined, Processes, Files (I/O)</t>
+  </si>
+  <si>
+    <t>Functions, Globals, Stack, Output, Files (I/O)</t>
+  </si>
+  <si>
+    <t>Arguments, Commands, Platform, Env. Var.</t>
+  </si>
+  <si>
+    <t>User defined, Stack Trace, Platform, Source</t>
+  </si>
+  <si>
+    <t>Blocks, Calls, Random Seed, User Input</t>
+  </si>
+  <si>
+    <t>Functions, Variables, Env. Var., Platform, Modules, Files (I/O)</t>
+  </si>
+  <si>
+    <t>Language Constructs, Files (I/O)</t>
+  </si>
+  <si>
+    <t>Arguments, Output, Sumatra</t>
+  </si>
+  <si>
+    <t>Commands, Variables, Values, Env. Var., Platform, Modules, Files (I/O)</t>
+  </si>
+  <si>
+    <t>User defined, Output, Modules, Host, Source, Files (I/O)</t>
+  </si>
+  <si>
+    <t>User defined, Files (I/O), Source</t>
+  </si>
+  <si>
+    <t>Functions, Returns, Arguments, Stack Trace</t>
+  </si>
+  <si>
+    <t>Functions, Modules, Files (I/O), Stack Trace</t>
+  </si>
+  <si>
+    <t>Modules, Files (I/O)</t>
+  </si>
+  <si>
+    <t>Arguments, Output, Source</t>
+  </si>
+  <si>
+    <t>User defined, Variables, Calls, Stack Trace</t>
+  </si>
+  <si>
+    <t>Processes, Modules, Files (I/O - metadata)</t>
+  </si>
+  <si>
     <t>User defined</t>
   </si>
   <si>
-    <t>User defined, Env. Var.</t>
-  </si>
-  <si>
-    <t>Commands, Variables, Random Seed, Files (I)</t>
-  </si>
-  <si>
-    <t>User defined, Parameters, Platform, Modules, Source</t>
-  </si>
-  <si>
-    <t>Files (I/O - metadata)</t>
-  </si>
-  <si>
-    <t>User defined, Processes, Files (I/O)</t>
-  </si>
-  <si>
-    <t>Functions, Globals, Stack, Output, Files (I/O)</t>
-  </si>
-  <si>
-    <t>Arguments, Commands, Platform, Env. Var.</t>
-  </si>
-  <si>
-    <t>User defined, Stack Trace, Platform, Source</t>
-  </si>
-  <si>
-    <t>Blocks, Calls, Random Seed, User Input</t>
-  </si>
-  <si>
-    <t>Functions, Variables, Env. Var., Platform, Modules, Files (I/O)</t>
-  </si>
-  <si>
-    <t>Language Constructs, Files (I/O)</t>
-  </si>
-  <si>
-    <t>Arguments, Output, Sumatra</t>
-  </si>
-  <si>
-    <t>Commands, Variables, Values</t>
-  </si>
-  <si>
-    <t>User defined, Output, Modules, Host, Source, Files (I/O)</t>
-  </si>
-  <si>
-    <t>User defined, Files (I/O), Source</t>
-  </si>
-  <si>
-    <t>Functions, Modules, Files (I/O), Stack Trace</t>
-  </si>
-  <si>
-    <t>Modules, Files (I/O)</t>
-  </si>
-  <si>
-    <t>Functions, Returns, Arguments, Stack Trace</t>
-  </si>
-  <si>
-    <t>Arguments, Output, Source</t>
-  </si>
-  <si>
-    <t>User defined, Variables, Calls, Stack Trace</t>
-  </si>
-  <si>
-    <t>Processes, Modules, Files (I/O - metadata)</t>
-  </si>
-  <si>
     <t>Variables, Dependencies, User defined</t>
   </si>
   <si>
     <t>Inte</t>
   </si>
   <si>
+    <t>Inte, Exte</t>
+  </si>
+  <si>
     <t>Pars, Exec</t>
+  </si>
+  <si>
+    <t>Defi, Prov</t>
+  </si>
+  <si>
+    <t>Man, Opt</t>
   </si>
   <si>
     <t>every activity</t>
@@ -798,37 +819,37 @@
         <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="L2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="M2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="O2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="P2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="Q2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="R2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -860,7 +881,7 @@
         <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K3" t="s">
         <v>36</v>
@@ -872,7 +893,7 @@
         <v>36</v>
       </c>
       <c r="N3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O3" t="s">
         <v>36</v>
@@ -910,10 +931,10 @@
         <v>46</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J4" t="s">
         <v>36</v>
@@ -931,7 +952,7 @@
         <v>36</v>
       </c>
       <c r="O4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P4" t="s">
         <v>36</v>
@@ -963,13 +984,13 @@
         <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J5" t="s">
         <v>36</v>
@@ -978,13 +999,13 @@
         <v>36</v>
       </c>
       <c r="L5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O5" t="s">
         <v>36</v>
@@ -1025,7 +1046,7 @@
         <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J6" t="s">
         <v>36</v>
@@ -1037,10 +1058,10 @@
         <v>36</v>
       </c>
       <c r="M6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O6" t="s">
         <v>36</v>
@@ -1084,7 +1105,7 @@
         <v>36</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K7" t="s">
         <v>36</v>
@@ -1134,13 +1155,13 @@
         <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I8" t="s">
         <v>36</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K8" t="s">
         <v>36</v>
@@ -1187,22 +1208,22 @@
         <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I9" t="s">
         <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K9" t="s">
         <v>36</v>
       </c>
       <c r="L9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M9" t="s">
         <v>36</v>
@@ -1243,16 +1264,16 @@
         <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K10" t="s">
         <v>36</v>
@@ -1264,7 +1285,7 @@
         <v>36</v>
       </c>
       <c r="N10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O10" t="s">
         <v>36</v>
@@ -1305,7 +1326,7 @@
         <v>36</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J11" t="s">
         <v>36</v>
@@ -1317,10 +1338,10 @@
         <v>36</v>
       </c>
       <c r="M11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O11" t="s">
         <v>36</v>
@@ -1355,13 +1376,13 @@
         <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J12" t="s">
         <v>36</v>
@@ -1370,13 +1391,13 @@
         <v>36</v>
       </c>
       <c r="L12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O12" t="s">
         <v>36</v>
@@ -1411,13 +1432,13 @@
         <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J13" t="s">
         <v>36</v>
@@ -1426,7 +1447,7 @@
         <v>36</v>
       </c>
       <c r="L13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M13" t="s">
         <v>36</v>
@@ -1473,7 +1494,7 @@
         <v>36</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J14" t="s">
         <v>36</v>
@@ -1485,10 +1506,10 @@
         <v>36</v>
       </c>
       <c r="M14" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N14" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O14" t="s">
         <v>36</v>
@@ -1532,7 +1553,7 @@
         <v>36</v>
       </c>
       <c r="J15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K15" t="s">
         <v>36</v>
@@ -1579,13 +1600,13 @@
         <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J16" t="s">
         <v>36</v>
@@ -1594,7 +1615,7 @@
         <v>36</v>
       </c>
       <c r="L16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M16" t="s">
         <v>36</v>
@@ -1700,51 +1721,51 @@
         <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="L2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="M2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="O2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="P2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="Q2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="R2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -1753,10 +1774,10 @@
         <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
         <v>36</v>
@@ -1768,7 +1789,7 @@
         <v>36</v>
       </c>
       <c r="L3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M3" t="s">
         <v>36</v>
@@ -1777,7 +1798,7 @@
         <v>36</v>
       </c>
       <c r="O3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P3" t="s">
         <v>36</v>
@@ -1786,18 +1807,18 @@
         <v>36</v>
       </c>
       <c r="R3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
         <v>36</v>
@@ -1818,7 +1839,7 @@
         <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K4" t="s">
         <v>36</v>
@@ -1842,21 +1863,21 @@
         <v>36</v>
       </c>
       <c r="R4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
         <v>40</v>
@@ -1865,10 +1886,10 @@
         <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I5" t="s">
         <v>36</v>
@@ -1880,16 +1901,16 @@
         <v>36</v>
       </c>
       <c r="L5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M5" t="s">
         <v>36</v>
       </c>
       <c r="N5" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="O5" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="P5" t="s">
         <v>36</v>
@@ -1898,27 +1919,27 @@
         <v>36</v>
       </c>
       <c r="R5" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
         <v>36</v>
@@ -1936,13 +1957,13 @@
         <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="M6" t="s">
         <v>36</v>
       </c>
       <c r="N6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="O6" t="s">
         <v>36</v>
@@ -1959,13 +1980,13 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
@@ -1986,7 +2007,7 @@
         <v>36</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K7" t="s">
         <v>36</v>
@@ -2015,16 +2036,16 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -2033,10 +2054,10 @@
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>121</v>
       </c>
       <c r="I8" t="s">
         <v>36</v>
@@ -2048,16 +2069,16 @@
         <v>36</v>
       </c>
       <c r="L8" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M8" t="s">
         <v>36</v>
       </c>
       <c r="N8" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="P8" t="s">
         <v>36</v>
@@ -2066,7 +2087,7 @@
         <v>36</v>
       </c>
       <c r="R8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -2077,7 +2098,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
         <v>36</v>
@@ -2098,7 +2119,7 @@
         <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K9" t="s">
         <v>36</v>
@@ -2127,16 +2148,16 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
@@ -2145,10 +2166,10 @@
         <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
         <v>36</v>
@@ -2160,7 +2181,7 @@
         <v>36</v>
       </c>
       <c r="L10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M10" t="s">
         <v>36</v>
@@ -2169,7 +2190,7 @@
         <v>36</v>
       </c>
       <c r="O10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P10" t="s">
         <v>36</v>
@@ -2178,21 +2199,21 @@
         <v>36</v>
       </c>
       <c r="R10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -2201,22 +2222,22 @@
         <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I11" t="s">
         <v>36</v>
       </c>
       <c r="J11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K11" t="s">
         <v>36</v>
       </c>
       <c r="L11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M11" t="s">
         <v>36</v>
@@ -2225,30 +2246,30 @@
         <v>36</v>
       </c>
       <c r="O11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="Q11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
@@ -2257,10 +2278,10 @@
         <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I12" t="s">
         <v>36</v>
@@ -2272,10 +2293,10 @@
         <v>36</v>
       </c>
       <c r="L12" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="M12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N12" t="s">
         <v>36</v>
@@ -2284,10 +2305,10 @@
         <v>36</v>
       </c>
       <c r="P12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="Q12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R12" t="s">
         <v>36</v>
@@ -2295,16 +2316,16 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -2313,10 +2334,10 @@
         <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I13" t="s">
         <v>36</v>
@@ -2328,22 +2349,22 @@
         <v>36</v>
       </c>
       <c r="L13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M13" t="s">
         <v>36</v>
       </c>
       <c r="N13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="O13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P13" t="s">
         <v>36</v>
       </c>
       <c r="Q13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R13" t="s">
         <v>36</v>
@@ -2351,13 +2372,13 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D14" t="s">
         <v>36</v>
@@ -2378,7 +2399,7 @@
         <v>36</v>
       </c>
       <c r="J14" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K14" t="s">
         <v>36</v>
@@ -2402,18 +2423,18 @@
         <v>36</v>
       </c>
       <c r="R14" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D15" t="s">
         <v>36</v>
@@ -2431,10 +2452,10 @@
         <v>36</v>
       </c>
       <c r="I15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K15" t="s">
         <v>36</v>
@@ -2443,33 +2464,33 @@
         <v>36</v>
       </c>
       <c r="M15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N15" t="s">
         <v>36</v>
       </c>
       <c r="O15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="Q15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R15" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -2481,10 +2502,10 @@
         <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H16" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I16" t="s">
         <v>36</v>
@@ -2493,7 +2514,7 @@
         <v>36</v>
       </c>
       <c r="K16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="L16" t="s">
         <v>36</v>
@@ -2508,10 +2529,10 @@
         <v>36</v>
       </c>
       <c r="P16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="Q16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R16" t="s">
         <v>36</v>
@@ -2519,16 +2540,16 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
         <v>40</v>
@@ -2537,10 +2558,10 @@
         <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>121</v>
       </c>
       <c r="I17" t="s">
         <v>36</v>
@@ -2552,22 +2573,22 @@
         <v>36</v>
       </c>
       <c r="L17" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M17" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N17" t="s">
         <v>36</v>
       </c>
       <c r="O17" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P17" t="s">
         <v>36</v>
       </c>
       <c r="Q17" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R17" t="s">
         <v>36</v>
@@ -2575,22 +2596,22 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D18" t="s">
-        <v>113</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G18" t="s">
         <v>36</v>
@@ -2599,25 +2620,25 @@
         <v>36</v>
       </c>
       <c r="I18" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J18" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="K18" t="s">
         <v>36</v>
       </c>
       <c r="L18" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="M18" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="N18" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="O18" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="P18" t="s">
         <v>36</v>
@@ -2626,21 +2647,21 @@
         <v>36</v>
       </c>
       <c r="R18" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D19" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -2649,51 +2670,51 @@
         <v>42</v>
       </c>
       <c r="G19" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="I19" t="s">
         <v>36</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="K19" t="s">
         <v>36</v>
       </c>
       <c r="L19" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M19" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N19" t="s">
         <v>36</v>
       </c>
       <c r="O19" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P19" t="s">
         <v>36</v>
       </c>
       <c r="Q19" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R19" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D20" t="s">
         <v>37</v>
@@ -2708,7 +2729,7 @@
         <v>46</v>
       </c>
       <c r="H20" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I20" t="s">
         <v>36</v>
@@ -2720,7 +2741,7 @@
         <v>36</v>
       </c>
       <c r="L20" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M20" t="s">
         <v>36</v>
@@ -2729,13 +2750,13 @@
         <v>36</v>
       </c>
       <c r="O20" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P20" t="s">
         <v>36</v>
       </c>
       <c r="Q20" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R20" t="s">
         <v>36</v>
@@ -2743,34 +2764,34 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D21" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I21" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="J21" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="K21" t="s">
         <v>36</v>
@@ -2779,7 +2800,7 @@
         <v>36</v>
       </c>
       <c r="M21" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N21" t="s">
         <v>36</v>
@@ -2788,10 +2809,10 @@
         <v>36</v>
       </c>
       <c r="P21" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="Q21" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="R21" t="s">
         <v>36</v>
@@ -2799,69 +2820,69 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="F22" t="s">
         <v>42</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I22" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="J22" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="K22" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="L22" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="M22" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N22" t="s">
         <v>36</v>
       </c>
       <c r="O22" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="P22" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="Q22" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R22" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D23" t="s">
         <v>37</v>
@@ -2870,40 +2891,40 @@
         <v>39</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G23" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H23" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I23" t="s">
         <v>36</v>
       </c>
       <c r="J23" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="K23" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="L23" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="M23" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="N23" t="s">
         <v>36</v>
       </c>
       <c r="O23" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="P23" t="s">
         <v>36</v>
       </c>
       <c r="Q23" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="R23" t="s">
         <v>36</v>
@@ -2911,13 +2932,13 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D24" t="s">
         <v>37</v>
@@ -2932,7 +2953,7 @@
         <v>46</v>
       </c>
       <c r="H24" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I24" t="s">
         <v>36</v>
@@ -2941,7 +2962,7 @@
         <v>36</v>
       </c>
       <c r="K24" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="L24" t="s">
         <v>36</v>
@@ -2953,13 +2974,13 @@
         <v>36</v>
       </c>
       <c r="O24" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P24" t="s">
         <v>36</v>
       </c>
       <c r="Q24" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R24" t="s">
         <v>36</v>
@@ -2967,16 +2988,16 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E25" t="s">
         <v>40</v>
@@ -2985,10 +3006,10 @@
         <v>42</v>
       </c>
       <c r="G25" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H25" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I25" t="s">
         <v>36</v>
@@ -3000,7 +3021,7 @@
         <v>36</v>
       </c>
       <c r="L25" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M25" t="s">
         <v>36</v>
@@ -3023,16 +3044,16 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E26" t="s">
         <v>40</v>
@@ -3041,10 +3062,10 @@
         <v>42</v>
       </c>
       <c r="G26" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H26" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I26" t="s">
         <v>36</v>
@@ -3056,7 +3077,7 @@
         <v>36</v>
       </c>
       <c r="L26" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M26" t="s">
         <v>36</v>
@@ -3065,69 +3086,69 @@
         <v>36</v>
       </c>
       <c r="O26" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P26" t="s">
         <v>36</v>
       </c>
       <c r="Q26" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R26" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G27" t="s">
         <v>36</v>
       </c>
       <c r="H27" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="I27" t="s">
         <v>36</v>
       </c>
       <c r="J27" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K27" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="L27" t="s">
         <v>36</v>
       </c>
       <c r="M27" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N27" t="s">
         <v>36</v>
       </c>
       <c r="O27" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P27" t="s">
         <v>36</v>
       </c>
       <c r="Q27" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R27" t="s">
         <v>36</v>
@@ -3135,16 +3156,16 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="D28" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E28" t="s">
         <v>39</v>
@@ -3153,10 +3174,10 @@
         <v>42</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H28" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I28" t="s">
         <v>36</v>
@@ -3165,10 +3186,10 @@
         <v>36</v>
       </c>
       <c r="K28" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="L28" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M28" t="s">
         <v>36</v>
@@ -3191,16 +3212,16 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D29" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E29" t="s">
         <v>39</v>
@@ -3209,40 +3230,40 @@
         <v>42</v>
       </c>
       <c r="G29" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H29" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="K29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="L29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N29" t="s">
         <v>36</v>
       </c>
       <c r="O29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="P29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="Q29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="R29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add changes based on authors' replies
</commit_message>
<xml_diff>
--- a/notebooks/output/gathering.xlsx
+++ b/notebooks/output/gathering.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="124">
   <si>
     <t>Annotations</t>
   </si>
@@ -185,10 +185,10 @@
     <t>Instrumentation</t>
   </si>
   <si>
-    <t>Before</t>
-  </si>
-  <si>
-    <t>During</t>
+    <t>Snapshot</t>
+  </si>
+  <si>
+    <t>Continuous</t>
   </si>
   <si>
     <t>Reading</t>
@@ -344,7 +344,7 @@
     <t>User defined, Files (I/O), Source</t>
   </si>
   <si>
-    <t>Functions, Returns, Arguments, Stack Trace</t>
+    <t>Functions, Returns, Arguments, Stack Trace, Env. Var.</t>
   </si>
   <si>
     <t>Functions, Modules, Files (I/O), Stack Trace</t>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>Inte</t>
+  </si>
+  <si>
+    <t>—</t>
   </si>
   <si>
     <t>Inte, Exte</t>
@@ -1933,49 +1936,49 @@
         <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="L6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="M6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="N6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="O6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="P6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="Q6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="R6" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -2054,10 +2057,10 @@
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I8" t="s">
         <v>36</v>
@@ -2558,10 +2561,10 @@
         <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I17" t="s">
         <v>36</v>
@@ -2832,7 +2835,7 @@
         <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F22" t="s">
         <v>42</v>
@@ -3130,7 +3133,7 @@
         <v>52</v>
       </c>
       <c r="K27" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L27" t="s">
         <v>36</v>
@@ -3165,7 +3168,7 @@
         <v>115</v>
       </c>
       <c r="D28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E28" t="s">
         <v>39</v>

</xml_diff>